<commit_message>
update xlsx for network
</commit_message>
<xml_diff>
--- a/ragdoll/core/NUTR_DEF_more1.xlsx
+++ b/ragdoll/core/NUTR_DEF_more1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="营养素类别" sheetId="2" r:id="rId2"/>
     <sheet name="foodmate" sheetId="3" r:id="rId3"/>
     <sheet name="cnsoc" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="975">
   <si>
     <t>code</t>
   </si>
@@ -2496,16 +2497,671 @@
   <si>
     <t>生物素</t>
   </si>
+  <si>
+    <t>MACC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monosaccharide</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DACC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disaccharide</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PACC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polysaccharide</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBH</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glucose</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carbohydrate</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dietary Fiber</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mineral</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calcium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sodium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potassium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zinc</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copper</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Selenium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iodine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manganese</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Molybdenum</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chromium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MNL</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magnesium</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZN</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CU</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SE</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fluorine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CR</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Protein</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROCNT</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amino Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indispensable Amino Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conditionally Indispensable Amino Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dispensable Amino Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isoleucine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leucine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lysine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Methionine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phenylanine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Threonine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tryptophan</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Histidine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glycine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arginine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glutamine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proline</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cystine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tryosine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taurine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ornithine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Citrulline</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glutamic Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alanine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Serine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aspartic Acid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asparagine</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>IAA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIAA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAA</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>VAL_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILE_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEU_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LYS_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MET_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHE_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>THR_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRP_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>HISTN_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLY_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARG_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLN_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CYS_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TYR_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAU_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORN_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CIT_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLU_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALA_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SER_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASP_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASPG_G</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIP</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lipid</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fatty acids, saturated</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fatty acids, monounsaturated</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体 (Body)"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Fatty acids</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, polyunsaturated</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitamin</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIT</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F22D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F15D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F17D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F24D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F13D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F18D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F14D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F16D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F20D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>24:1 c</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F4D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F15D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F17D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F22D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F24D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>24:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:6</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F18D2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F18D3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F18D4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F20D3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F20D4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F20D5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F21D5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F22D4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F22D5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F22D6</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F18D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>3:0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>2:0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F3D0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F12D1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>21:5</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAMNUS</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAPLUS</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -2547,13 +3203,116 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体 (Body)"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2580,29 +3339,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2902,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3468,15 +4255,6 @@
       <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F20" s="4" t="s">
         <v>110</v>
       </c>
@@ -3497,15 +4275,6 @@
       <c r="B21" t="s">
         <v>112</v>
       </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F21" s="4" t="s">
         <v>115</v>
       </c>
@@ -7290,7 +8059,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7299,8 +8068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173:D176"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -8264,7 +9033,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
@@ -8814,7 +9583,7 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A29:A37"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
@@ -8824,7 +9593,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -9162,7 +9931,877 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="176" zoomScalePageLayoutView="176" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A2" s="25" t="s">
+        <v>824</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>818</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>820</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>822</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A14" s="25" t="s">
+        <v>859</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>858</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>887</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>860</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>888</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>861</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>889</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>862</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>890</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>891</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>892</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>893</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>894</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>895</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>896</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>897</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>898</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>899</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>900</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>901</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>902</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>903</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>876</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="N31" s="11" t="s">
+        <v>927</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>904</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>905</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>906</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>907</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>908</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>909</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>910</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>911</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>884</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>841</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>912</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>885</v>
+      </c>
+      <c r="E40" t="s">
+        <v>842</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>913</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>886</v>
+      </c>
+      <c r="E41" t="s">
+        <v>845</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>447</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="E42" t="s">
+        <v>846</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A43" s="25" t="s">
+        <v>914</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>915</v>
+      </c>
+      <c r="E43" t="s">
+        <v>847</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>472</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>916</v>
+      </c>
+      <c r="E44" t="s">
+        <v>848</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>973</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>917</v>
+      </c>
+      <c r="E45" t="s">
+        <v>849</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="16" t="s">
+        <v>974</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>918</v>
+      </c>
+      <c r="E46" t="s">
+        <v>850</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="18" t="s">
+        <v>961</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>960</v>
+      </c>
+      <c r="E47" t="s">
+        <v>851</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="18" t="s">
+        <v>962</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>959</v>
+      </c>
+      <c r="E48" t="s">
+        <v>852</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A49" s="18" t="s">
+        <v>963</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>958</v>
+      </c>
+      <c r="E49" t="s">
+        <v>853</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A50" s="18" t="s">
+        <v>938</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="E50" t="s">
+        <v>844</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A51" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="E51" t="s">
+        <v>854</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A52" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>488</v>
+      </c>
+      <c r="E52" t="s">
+        <v>855</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>856</v>
+      </c>
+      <c r="L52" s="17" t="s">
+        <v>633</v>
+      </c>
+      <c r="M52" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A53" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="E53" t="s">
+        <v>857</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A54" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="L54" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>683</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A55" s="18" t="s">
+        <v>932</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A56" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="M56" s="17" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A57" s="18" t="s">
+        <v>929</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A58" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>653</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="N58" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O58" s="17" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A59" s="18" t="s">
+        <v>930</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>623</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>753</v>
+      </c>
+      <c r="M59" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="N59" s="17" t="s">
+        <v>673</v>
+      </c>
+      <c r="O59" s="17" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A60" s="18" t="s">
+        <v>957</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A61" s="18" t="s">
+        <v>517</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A62" s="18" t="s">
+        <v>928</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="L62" s="17" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A63" s="18" t="s">
+        <v>931</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>628</v>
+      </c>
+      <c r="L63" s="17" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A64" s="11" t="s">
+        <v>969</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A65" s="11" t="s">
+        <v>934</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A66" s="11" t="s">
+        <v>939</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>967</v>
+      </c>
+      <c r="L66" s="17" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A67" s="11" t="s">
+        <v>935</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>920</v>
+      </c>
+      <c r="L67" s="17" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A68" s="11" t="s">
+        <v>940</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A69" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A70" s="11" t="s">
+        <v>936</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A71" s="11" t="s">
+        <v>941</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A72" s="11" t="s">
+        <v>942</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A73" s="23" t="s">
+        <v>947</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A74" s="23" t="s">
+        <v>948</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A75" s="23" t="s">
+        <v>949</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A76" s="23" t="s">
+        <v>950</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A77" s="23" t="s">
+        <v>951</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A78" s="23" t="s">
+        <v>952</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A79" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A80" s="23" t="s">
+        <v>954</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81" s="23" t="s">
+        <v>955</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82" s="23" t="s">
+        <v>956</v>
+      </c>
+      <c r="B82" s="24" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F91" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>